<commit_message>
Archivos creacion BD desde cero segun rubrica
</commit_message>
<xml_diff>
--- a/RubricaPlitix_SQLWarriors.xlsx
+++ b/RubricaPlitix_SQLWarriors.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alcaz\Git\ProyectoABD-SQLWarriors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F33A068-E770-416B-BD20-CBD4E4AA9B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1F4BEE2-280E-4791-8CD7-F3F014EEDFC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="X7LfdmuZ3ss+actbBwJKlGQw0Mfe8mdGrYC6BLVbRaWZI0OVWK1VPKEuVw1nyVdQeaaH9MAmoO0Rse/4Wdr3PA==" workbookSaltValue="2gPJKYWhIGazIFYGx/RJog==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="50895" yWindow="-7245" windowWidth="12810" windowHeight="15855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="3" r:id="rId1"/>
@@ -847,8 +847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C334588-D4EB-43EC-8424-5ED08F8B2503}">
   <dimension ref="A1:U61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -969,12 +969,12 @@
         <v>49</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
@@ -983,12 +983,12 @@
         <v>69</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9">
         <f>IF(D9="SI",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
@@ -1003,12 +1003,12 @@
         <v>41</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
@@ -1051,12 +1051,12 @@
         <v>76</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E13" s="12"/>
       <c r="F13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
@@ -1372,12 +1372,12 @@
         <v>20</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E33" s="12"/>
       <c r="F33">
         <f t="shared" ref="F33:F38" si="1">IF(D33="SI",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.3">
@@ -1457,7 +1457,7 @@
       <c r="E39" s="9"/>
       <c r="F39" s="11">
         <f>SUM(F6:F38)/COUNT(F6:F38)*2</f>
-        <v>0.30303030303030304</v>
+        <v>0.48484848484848486</v>
       </c>
     </row>
     <row r="40" spans="1:20" ht="23.4" x14ac:dyDescent="0.45">
@@ -1759,7 +1759,7 @@
       <c r="C60" s="5"/>
       <c r="F60" s="10">
         <f>F59+F39</f>
-        <v>0.30303030303030304</v>
+        <v>0.48484848484848486</v>
       </c>
       <c r="G60" s="10"/>
       <c r="H60" s="10"/>

</xml_diff>

<commit_message>
Actualizacion creacionBD hasta permisos
</commit_message>
<xml_diff>
--- a/RubricaPlitix_SQLWarriors.xlsx
+++ b/RubricaPlitix_SQLWarriors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alcaz\Git\ProyectoABD-SQLWarriors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1F4BEE2-280E-4791-8CD7-F3F014EEDFC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C17ED7-45E3-4DF8-ABEA-644FE13E707C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="X7LfdmuZ3ss+actbBwJKlGQw0Mfe8mdGrYC6BLVbRaWZI0OVWK1VPKEuVw1nyVdQeaaH9MAmoO0Rse/4Wdr3PA==" workbookSaltValue="2gPJKYWhIGazIFYGx/RJog==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -847,8 +847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C334588-D4EB-43EC-8424-5ED08F8B2503}">
   <dimension ref="A1:U61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1017,12 +1017,12 @@
         <v>42</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
@@ -1037,12 +1037,12 @@
         <v>50</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
@@ -1334,12 +1334,12 @@
         <v>31</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E31" s="12"/>
       <c r="F31">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1442,12 +1442,12 @@
         <v>33</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E38" s="12"/>
       <c r="F38">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.3">
@@ -1457,7 +1457,7 @@
       <c r="E39" s="9"/>
       <c r="F39" s="11">
         <f>SUM(F6:F38)/COUNT(F6:F38)*2</f>
-        <v>0.48484848484848486</v>
+        <v>0.60606060606060608</v>
       </c>
     </row>
     <row r="40" spans="1:20" ht="23.4" x14ac:dyDescent="0.45">
@@ -1759,7 +1759,7 @@
       <c r="C60" s="5"/>
       <c r="F60" s="10">
         <f>F59+F39</f>
-        <v>0.48484848484848486</v>
+        <v>0.60606060606060608</v>
       </c>
       <c r="G60" s="10"/>
       <c r="H60" s="10"/>

</xml_diff>

<commit_message>
Añadiendo evidencias para comprobar
</commit_message>
<xml_diff>
--- a/RubricaPlitix_SQLWarriors.xlsx
+++ b/RubricaPlitix_SQLWarriors.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28926"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alcaz\Git\ProyectoABD-SQLWarriors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D1B2713-2C9C-40BD-BF43-3E48F8A04DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8BF8A3D-951D-4207-A3A0-27400270EA57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="X7LfdmuZ3ss+actbBwJKlGQw0Mfe8mdGrYC6BLVbRaWZI0OVWK1VPKEuVw1nyVdQeaaH9MAmoO0Rse/4Wdr3PA==" workbookSaltValue="2gPJKYWhIGazIFYGx/RJog==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="50904" yWindow="-7248" windowWidth="12792" windowHeight="15852" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="15552" windowHeight="17376" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="3" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,6 +30,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -40,7 +41,256 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="92">
+  <si>
+    <t>Nombre del Grupo:</t>
+  </si>
+  <si>
+    <t>Integrantes  que han colaborado en el trabajo en orden alfabético de apellidos:</t>
+  </si>
+  <si>
+    <t>Grupo</t>
+  </si>
+  <si>
+    <t>Elementos</t>
+  </si>
+  <si>
+    <t>Realizado (SI/NO)</t>
+  </si>
+  <si>
+    <t>Evidencias: Dónde debe mirar el profesor para comprobar que se ha hecho</t>
+  </si>
+  <si>
+    <t>Nota:</t>
+  </si>
+  <si>
+    <t>¿Se han creado los siguientes objetos?</t>
+  </si>
+  <si>
+    <t>¿Se ha creado un esquema distinto para el trabajo?</t>
+  </si>
+  <si>
+    <t>Se ha creado el tablespace independiente TS_PLYTIX y TS_INDICES para el trabajo?</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>Consultar la vista dba_tablespaces</t>
+  </si>
+  <si>
+    <t>Se han creado índices en la base de datos? De qué tipo? Porqué? Cuales?</t>
+  </si>
+  <si>
+    <t>Consultar la vista user_indexes</t>
+  </si>
+  <si>
+    <t>¿Se han importado los datos a la tablas Cuentas, Planes, Usuarios, Productos tal y como se especificaba en la práctica de nivel físico? ¿Se ha creado la tabla externa?</t>
+  </si>
+  <si>
+    <t>Consultar las 4 tablas para ver si los datos están importados correctamente. Consultar la vista user_external_tables para ver la tabla externa</t>
+  </si>
+  <si>
+    <t>¿Se ha creado la tabla TRAZA y se usa para seguir errores?</t>
+  </si>
+  <si>
+    <t>Consultar la tabla traza</t>
+  </si>
+  <si>
+    <t>Seguridad</t>
+  </si>
+  <si>
+    <t>¿Se ha cifrado alguna columna como se indicaba en la práctica de seguridad?</t>
+  </si>
+  <si>
+    <t>Consultar la vista dba_encrypted_columns</t>
+  </si>
+  <si>
+    <t>¿Se ha aplicado alguna política de autorización VPD?</t>
+  </si>
+  <si>
+    <t>Consultar la vista dba_policies</t>
+  </si>
+  <si>
+    <t>Vistas</t>
+  </si>
+  <si>
+    <t>V_PRODUCTO_PUBLICO</t>
+  </si>
+  <si>
+    <t>Consultar la vista user_views</t>
+  </si>
+  <si>
+    <t>Materializada: VM_PRODUCTOS</t>
+  </si>
+  <si>
+    <t>Consultar la vista user_mviews</t>
+  </si>
+  <si>
+    <t>Permisos</t>
+  </si>
+  <si>
+    <t>Gestión de Productos por Usuario Estándar</t>
+  </si>
+  <si>
+    <t>Gestión de Productos, Activos y Categorías</t>
+  </si>
+  <si>
+    <t>Gestión de Atributos y Relaciones entre Productos</t>
+  </si>
+  <si>
+    <t>Gestión de las Cuentas</t>
+  </si>
+  <si>
+    <t>Gestión de los Planes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paquetes PL/SQL </t>
+  </si>
+  <si>
+    <t>PKG_ADMIN_PRODUCTOS</t>
+  </si>
+  <si>
+    <t>Consultar la vista user_objects</t>
+  </si>
+  <si>
+    <t>Procedimientos (dentro del paquete)</t>
+  </si>
+  <si>
+    <t>F_OBTENER_PLAN_CUENTA</t>
+  </si>
+  <si>
+    <t>Consultar la vista user_source, consultado por el nombre de la función</t>
+  </si>
+  <si>
+    <t>F_CONTAR_PRODUCTOS_CUENTA</t>
+  </si>
+  <si>
+    <t>F_VALIDAR_ATRIBUTOS_PRODUCTO</t>
+  </si>
+  <si>
+    <t>F_NUM_CATEGORIAS_CUENTA</t>
+  </si>
+  <si>
+    <t>P_ACTUALIZAR_NOMBRE_PRODUCTO</t>
+  </si>
+  <si>
+    <t>Consultar la vista user_source, consultado por el nombre del procedimiento</t>
+  </si>
+  <si>
+    <t>P_ASOCIAR_ACTIVO_A_PRODUCTO</t>
+  </si>
+  <si>
+    <t>P_ELIMINAR_PRODUCTO_Y_ASOCIACIONES</t>
+  </si>
+  <si>
+    <t>P_CREAR_USUARIO</t>
+  </si>
+  <si>
+    <t>P_ACTUALIZAR_PRODUCTOS</t>
+  </si>
+  <si>
+    <t>Triggers</t>
+  </si>
+  <si>
+    <t>TR_PRODUCTOS</t>
+  </si>
+  <si>
+    <t>Consultar la vista user_triggers</t>
+  </si>
+  <si>
+    <t>Transacciones</t>
+  </si>
+  <si>
+    <t>Se han confirmado/deshecho las transacciones en los procedimientos y en los paquetes</t>
+  </si>
+  <si>
+    <t>Excepciones</t>
+  </si>
+  <si>
+    <t>Se han controlado excepciones</t>
+  </si>
+  <si>
+    <t>¿Se han probado todas las funcionalidades insertando datos coherentes?</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Se han creado  roles adecuadamente</t>
+  </si>
+  <si>
+    <t>Consultar la vista dba_roles</t>
+  </si>
+  <si>
+    <t>Se han asignado usuarios a los roles adecuadamente</t>
+  </si>
+  <si>
+    <t>Se han asignado los permisos de forma restrictiva a todos los usuarios. Ejemplos:</t>
+  </si>
+  <si>
+    <t>Operaciones a realizar por los usuarios</t>
+  </si>
+  <si>
+    <t>Alguna política de gestión de contraseñas</t>
+  </si>
+  <si>
+    <t>Se ha activado TDE y encriptado algunas columnas</t>
+  </si>
+  <si>
+    <t>Si has contestado NO a alguna de las pregunas anteriores, el trabajo se considera no superado</t>
+  </si>
+  <si>
+    <t>Si has contestado SI a todas las pregunas anteriores, y el trabajo está correcto, la nota del trabajo en grupo será 2 sobre 4</t>
+  </si>
+  <si>
+    <t>Para subir la nota se deben realizar las siguientes opciones:</t>
+  </si>
+  <si>
+    <t>Paquetes</t>
+  </si>
+  <si>
+    <t>PKG_ADMIN_PRODUCTOS_AVANZADO</t>
+  </si>
+  <si>
+    <t>F_VALIDAR_PLAN_SUFICIENTE</t>
+  </si>
+  <si>
+    <t>F_LISTA_CATEGORIAS_PRODUCTO</t>
+  </si>
+  <si>
+    <t>P_MIGRAR_PRODUCTOS_A_CATEGORIA</t>
+  </si>
+  <si>
+    <t>P_REPLICAR_ATRIBUTOS</t>
+  </si>
+  <si>
+    <t>JOBS</t>
+  </si>
+  <si>
+    <t>J_LIMPIA_TRAZA</t>
+  </si>
+  <si>
+    <t>Consultar la vista user_scheduler_jobs</t>
+  </si>
+  <si>
+    <t>J_ACTUALIZA_PRODUCTOS</t>
+  </si>
+  <si>
+    <t>¿Es el diseño (modelo E/R) de la base de datos correcto?</t>
+  </si>
+  <si>
+    <t>¿Se comprueban restricciones semánticas? El rango debe estar dentro de ..., números no negativos en ciertos campos, comparación de fechas, etc.</t>
+  </si>
+  <si>
+    <t>Se han creado Restricciones NOT NULL / UNIQUE</t>
+  </si>
+  <si>
+    <t>Auditoria</t>
+  </si>
+  <si>
+    <t>Se ha configurado AUDIT para modificación de planes o se ha creado un Trigger</t>
+  </si>
   <si>
     <t>Miscelanea</t>
   </si>
@@ -48,242 +298,32 @@
     <t>Se han introducido (SUFICIENTES) datos para comprobar la integridad referencial del modelo lógico?</t>
   </si>
   <si>
-    <t>Evidencias: Dónde debe mirar el profesor para comprobar que se ha hecho</t>
-  </si>
-  <si>
-    <t>Elementos</t>
-  </si>
-  <si>
-    <t>Nombre del Grupo:</t>
-  </si>
-  <si>
-    <t>Realizado (SI/NO)</t>
-  </si>
-  <si>
-    <t>SI</t>
-  </si>
-  <si>
-    <t>NO</t>
+    <t>Se han tratado correctamente las mayusculas/minusculas en triggers, índices, etc.</t>
+  </si>
+  <si>
+    <t>¿Se han introducido procedimientos/funciones/jobs/triggers o vistas adicionales a las propuestas?</t>
+  </si>
+  <si>
+    <t>Contexto</t>
+  </si>
+  <si>
+    <t>¿Se ha utilizado contexto de aplicaciones para distinguir el usuario activo y sus permisos?</t>
+  </si>
+  <si>
+    <t>Nota</t>
+  </si>
+  <si>
+    <t>Nota final</t>
   </si>
   <si>
     <t>Columna1</t>
-  </si>
-  <si>
-    <t>Si has contestado NO a alguna de las pregunas anteriores, el trabajo se considera no superado</t>
-  </si>
-  <si>
-    <t>Si has contestado SI a todas las pregunas anteriores, y el trabajo está correcto, la nota del trabajo en grupo será 2 sobre 4</t>
-  </si>
-  <si>
-    <t>Para subir la nota se deben realizar las siguientes opciones:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paquetes PL/SQL </t>
-  </si>
-  <si>
-    <t>Se han creado índices en la base de datos? De qué tipo? Porqué? Cuales?</t>
-  </si>
-  <si>
-    <t>¿Se ha creado un esquema distinto para el trabajo?</t>
-  </si>
-  <si>
-    <t>¿Se han probado todas las funcionalidades insertando datos coherentes?</t>
-  </si>
-  <si>
-    <t>¿Es el diseño (modelo E/R) de la base de datos correcto?</t>
-  </si>
-  <si>
-    <t>¿Se comprueban restricciones semánticas? El rango debe estar dentro de ..., números no negativos en ciertos campos, comparación de fechas, etc.</t>
-  </si>
-  <si>
-    <t>Se han creado Restricciones NOT NULL / UNIQUE</t>
-  </si>
-  <si>
-    <t>Seguridad</t>
-  </si>
-  <si>
-    <t>Se han creado  roles adecuadamente</t>
-  </si>
-  <si>
-    <t>Se han asignado usuarios a los roles adecuadamente</t>
-  </si>
-  <si>
-    <t>Se han asignado los permisos de forma restrictiva a todos los usuarios. Ejemplos:</t>
-  </si>
-  <si>
-    <t>Alguna política de gestión de contraseñas</t>
-  </si>
-  <si>
-    <t>Se han tratado correctamente las mayusculas/minusculas en triggers, índices, etc.</t>
-  </si>
-  <si>
-    <t>Transacciones</t>
-  </si>
-  <si>
-    <t>Auditoria</t>
-  </si>
-  <si>
-    <t>Vistas</t>
-  </si>
-  <si>
-    <t>¿Se han creado los siguientes objetos?</t>
-  </si>
-  <si>
-    <t>Triggers</t>
-  </si>
-  <si>
-    <t>Excepciones</t>
-  </si>
-  <si>
-    <t>Se han controlado excepciones</t>
-  </si>
-  <si>
-    <t>Se han confirmado/deshecho las transacciones en los procedimientos y en los paquetes</t>
-  </si>
-  <si>
-    <t>Se ha activado TDE y encriptado algunas columnas</t>
-  </si>
-  <si>
-    <t>¿Se han introducido procedimientos/funciones/jobs/triggers o vistas adicionales a las propuestas?</t>
-  </si>
-  <si>
-    <t>Integrantes  que han colaborado en el trabajo en orden alfabético de apellidos:</t>
-  </si>
-  <si>
-    <t>Nota</t>
-  </si>
-  <si>
-    <t>Nota final</t>
-  </si>
-  <si>
-    <t>Grupo</t>
-  </si>
-  <si>
-    <t>Nota:</t>
-  </si>
-  <si>
-    <t>Comprobar los tablespaces creados y los de las tablas e índices</t>
-  </si>
-  <si>
-    <t>¿Se ha cifrado alguna columna como se indicaba en la práctica de seguridad?</t>
-  </si>
-  <si>
-    <t>¿Se ha aplicado alguna política de autorización VPD?</t>
-  </si>
-  <si>
-    <t>Operaciones a realizar por los usuarios</t>
-  </si>
-  <si>
-    <t>Permisos</t>
-  </si>
-  <si>
-    <t>Paquetes</t>
-  </si>
-  <si>
-    <t>JOBS</t>
-  </si>
-  <si>
-    <t>Procedimientos (dentro del paquete)</t>
-  </si>
-  <si>
-    <t>Se ha creado el tablespace independiente TS_PLYTIX y TS_INDICES para el trabajo?</t>
-  </si>
-  <si>
-    <t>¿Se han importado los datos a la tablas Cuentas, Planes, Usuarios, Productos tal y como se especificaba en la práctica de nivel físico? ¿Se ha creado la tabla externa?</t>
-  </si>
-  <si>
-    <t>V_PRODUCTO_PUBLICO</t>
-  </si>
-  <si>
-    <t>Gestión de Productos, Activos y Categorías</t>
-  </si>
-  <si>
-    <t>Gestión de Atributos y Relaciones entre Productos</t>
-  </si>
-  <si>
-    <t>Gestión de las Cuentas</t>
-  </si>
-  <si>
-    <t>Gestión de los Planes</t>
-  </si>
-  <si>
-    <t>PKG_ADMIN_PRODUCTOS</t>
-  </si>
-  <si>
-    <t>F_OBTENER_PLAN_CUENTA</t>
-  </si>
-  <si>
-    <t>F_CONTAR_PRODUCTOS_CUENTA</t>
-  </si>
-  <si>
-    <t>F_VALIDAR_ATRIBUTOS_PRODUCTO</t>
-  </si>
-  <si>
-    <t>P_ACTUALIZAR_NOMBRE_PRODUCTO</t>
-  </si>
-  <si>
-    <t>P_ASOCIAR_ACTIVO_A_PRODUCTO</t>
-  </si>
-  <si>
-    <t>P_ELIMINAR_PRODUCTO_Y_ASOCIACIONES</t>
-  </si>
-  <si>
-    <t>P_CREAR_USUARIO</t>
-  </si>
-  <si>
-    <t>TR_PRODUCTOS</t>
-  </si>
-  <si>
-    <t>PKG_ADMIN_PRODUCTOS_AVANZADO</t>
-  </si>
-  <si>
-    <t>J_LIMPIA_TRAZA</t>
-  </si>
-  <si>
-    <t>Contexto</t>
-  </si>
-  <si>
-    <t>¿Se ha utilizado contexto de aplicaciones para distinguir el usuario activo y sus permisos?</t>
-  </si>
-  <si>
-    <t>Gestión de Productos por Usuario Estándar</t>
-  </si>
-  <si>
-    <t>¿Se ha creado la tabla TRAZA y se usa para seguir errores?</t>
-  </si>
-  <si>
-    <t>F_NUM_CATEGORIAS_CUENTA</t>
-  </si>
-  <si>
-    <t>P_ACTUALIZAR_PRODUCTOS</t>
-  </si>
-  <si>
-    <t>F_VALIDAR_PLAN_SUFICIENTE</t>
-  </si>
-  <si>
-    <t>P_MIGRAR_PRODUCTOS_A_CATEGORIA</t>
-  </si>
-  <si>
-    <t>P_REPLICAR_ATRIBUTOS</t>
-  </si>
-  <si>
-    <t>J_ACTUALIZA_PRODUCTOS</t>
-  </si>
-  <si>
-    <t>Materializada: VM_PRODUCTOS</t>
-  </si>
-  <si>
-    <t>F_LISTA_CATEGORIAS_PRODUCTO</t>
-  </si>
-  <si>
-    <t>Se ha configurado AUDIT para modificación de planes o se ha creado un Trigger</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -396,6 +436,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -537,30 +584,30 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -851,32 +898,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C334588-D4EB-43EC-8424-5ED08F8B2503}">
   <dimension ref="A1:U61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="B36" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="14.45"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="51.109375" customWidth="1"/>
-    <col min="3" max="3" width="46.109375" customWidth="1"/>
-    <col min="5" max="5" width="47.6640625" style="5" customWidth="1"/>
-    <col min="6" max="8" width="11.44140625" customWidth="1"/>
+    <col min="2" max="2" width="51.140625" customWidth="1"/>
+    <col min="3" max="3" width="46.140625" customWidth="1"/>
+    <col min="5" max="5" width="47.7109375" style="5" customWidth="1"/>
+    <col min="6" max="8" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21" ht="23.45">
       <c r="A1" s="7"/>
       <c r="B1" s="7" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C1" s="16"/>
       <c r="D1" s="7"/>
       <c r="E1" s="8"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="15.6">
       <c r="A2" s="17" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
@@ -884,30 +931,30 @@
       <c r="E2" s="15"/>
       <c r="F2" s="14"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="28.9">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>2</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -925,156 +972,170 @@
       <c r="T4" s="3"/>
       <c r="U4" s="3"/>
     </row>
-    <row r="5" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="15.6">
       <c r="B5" s="18" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="30.75">
       <c r="A6" s="19">
         <v>1</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="F6">
         <f t="shared" ref="F6:F32" si="0">IF(D6="SI",1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="30.75">
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="12"/>
       <c r="F7">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="60.75">
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>15</v>
+      </c>
       <c r="F8">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" ht="30.75">
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
-        <v>69</v>
+        <v>16</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>17</v>
+      </c>
       <c r="F9">
         <f>IF(D9="SI",1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="30.75">
       <c r="A10" s="19">
         <f>A6+1</f>
         <v>2</v>
       </c>
       <c r="B10" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>41</v>
-      </c>
       <c r="D10" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="F10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" ht="30.75">
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="30"/>
+        <v>10</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>22</v>
+      </c>
       <c r="F11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" ht="15.75">
       <c r="A12" s="19">
         <f>A10+1</f>
         <v>3</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>25</v>
+      </c>
       <c r="F12">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" ht="15">
       <c r="B13" s="5"/>
       <c r="C13" s="5" t="s">
-        <v>76</v>
+        <v>26</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="F13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" ht="15.6">
       <c r="A14" s="19">
         <v>4</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14">
@@ -1082,12 +1143,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21">
       <c r="C15" s="21" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E15" s="12"/>
       <c r="F15">
@@ -1095,13 +1156,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21">
       <c r="B16" s="5"/>
       <c r="C16" s="21" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16">
@@ -1109,13 +1170,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6">
       <c r="B17" s="5"/>
       <c r="C17" s="21" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17">
@@ -1123,13 +1184,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6">
       <c r="B18" s="5"/>
       <c r="C18" s="21" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18">
@@ -1137,188 +1198,208 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="15.75">
       <c r="A19" s="19">
         <v>5</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>36</v>
+      </c>
       <c r="F19">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="30.75">
       <c r="A20" s="19">
         <f>A19+1</f>
         <v>6</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>39</v>
+      </c>
       <c r="F20">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="30.75">
       <c r="B21" s="5"/>
       <c r="C21" s="22" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E21" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="E21" s="30" t="s">
+        <v>39</v>
+      </c>
       <c r="F21">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="30.75">
       <c r="B22" s="23"/>
       <c r="C22" s="22" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E22" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="E22" s="30" t="s">
+        <v>39</v>
+      </c>
       <c r="F22">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="30.75">
       <c r="B23" s="23"/>
       <c r="C23" s="22" t="s">
-        <v>70</v>
+        <v>42</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E23" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="E23" s="30" t="s">
+        <v>39</v>
+      </c>
       <c r="F23">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="30.75">
       <c r="B24" s="23"/>
       <c r="C24" s="24" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E24" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="E24" s="30" t="s">
+        <v>44</v>
+      </c>
       <c r="F24">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="25.9" customHeight="1">
       <c r="B25" s="23"/>
       <c r="C25" s="22" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>44</v>
+      </c>
       <c r="F25">
         <f>IF(D25="SI",1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6">
       <c r="C26" s="22" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F26">
         <f>IF(D26="SI",1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="25.9" customHeight="1">
       <c r="B27" s="23"/>
       <c r="C27" s="22" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E27" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="E27" s="30" t="s">
+        <v>44</v>
+      </c>
       <c r="F27">
         <f>IF(D27="SI",1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="25.9" customHeight="1">
       <c r="B28" s="23"/>
       <c r="C28" s="22" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>44</v>
+      </c>
       <c r="F28">
         <f>IF(D28="SI",1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="15.75">
       <c r="A29" s="19">
         <f>A20+1</f>
         <v>7</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E29" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="F29">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="28.9">
       <c r="A30" s="19">
         <f>A29+1</f>
         <v>8</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E30" s="12"/>
       <c r="F30">
@@ -1326,19 +1407,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="15.6">
       <c r="A31" s="19">
         <f>A30+1</f>
         <v>9</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E31" s="12"/>
       <c r="F31">
@@ -1346,17 +1427,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="15.6">
       <c r="A32" s="19">
         <f>A31+1</f>
         <v>10</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="13" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="E32" s="12"/>
       <c r="F32">
@@ -1364,33 +1445,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" ht="15.75">
       <c r="A33" s="19">
         <f>A32+1</f>
         <v>11</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>20</v>
+        <v>58</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E33" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>59</v>
+      </c>
       <c r="F33">
         <f t="shared" ref="F33:F38" si="1">IF(D33="SI",1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" ht="30.75">
       <c r="B34" s="5"/>
       <c r="C34" s="5" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="E34" s="12"/>
       <c r="F34">
@@ -1398,13 +1481,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" ht="28.9">
       <c r="B35" s="5"/>
       <c r="C35" s="5" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="E35" s="12"/>
       <c r="F35">
@@ -1412,13 +1495,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20">
       <c r="B36" s="5"/>
       <c r="C36" s="5" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="E36" s="12"/>
       <c r="F36">
@@ -1426,13 +1509,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20">
       <c r="B37" s="5"/>
       <c r="C37" s="5" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="E37" s="12"/>
       <c r="F37">
@@ -1440,13 +1523,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20">
       <c r="B38" s="5"/>
       <c r="C38" s="5" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="E38" s="12"/>
       <c r="F38">
@@ -1454,7 +1537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20">
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -1464,9 +1547,9 @@
         <v>1.6363636363636365</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:20" ht="23.45">
       <c r="B40" s="25" t="s">
-        <v>9</v>
+        <v>65</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
@@ -1486,157 +1569,171 @@
       <c r="S40" s="10"/>
       <c r="T40" s="10"/>
     </row>
-    <row r="41" spans="1:20" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:20" ht="23.45">
       <c r="B41" s="25" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="9"/>
     </row>
-    <row r="42" spans="1:20" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:20" ht="23.45">
       <c r="B42" s="25" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="9"/>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20">
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="9"/>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20">
       <c r="B44" s="5"/>
       <c r="E44" s="9"/>
     </row>
-    <row r="45" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" ht="15.6">
       <c r="A45" s="19">
         <v>1</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D45" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E45" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>36</v>
+      </c>
       <c r="F45">
         <f>IF(D45="SI",1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" ht="15.6">
       <c r="A46" s="17"/>
       <c r="B46" s="26"/>
       <c r="C46" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E46" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>39</v>
+      </c>
       <c r="F46">
         <f t="shared" ref="F46:F49" si="2">IF(D46="SI",1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" ht="15.6">
       <c r="A47" s="17"/>
       <c r="B47" s="26"/>
       <c r="C47" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E47" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>39</v>
+      </c>
       <c r="F47">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" ht="30.75">
       <c r="A48" s="17"/>
       <c r="B48" s="26"/>
       <c r="C48" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D48" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E48" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>44</v>
+      </c>
       <c r="F48">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:21" ht="30.75">
       <c r="A49" s="17"/>
       <c r="B49" s="26"/>
       <c r="C49" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E49" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>44</v>
+      </c>
       <c r="F49">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:21" ht="15.75">
       <c r="A50" s="19">
         <v>2</v>
       </c>
       <c r="B50" s="20" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E50" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="F50">
         <f t="shared" ref="F50:F58" si="3">IF(D50="SI",1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:21" ht="15.6">
       <c r="A51" s="26"/>
       <c r="B51" s="26"/>
       <c r="C51" s="5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D51" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E51" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="E51" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="F51">
         <f t="shared" ref="F51" si="4">IF(D51="SI",1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:21" ht="43.15">
       <c r="A52" s="19">
         <v>3</v>
       </c>
       <c r="B52" s="27" t="s">
-        <v>16</v>
+        <v>78</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="E52" s="12"/>
       <c r="F52">
@@ -1644,13 +1741,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:21">
       <c r="B53" s="5"/>
       <c r="C53" s="28" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="D53" s="13" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="E53" s="12"/>
       <c r="F53">
@@ -1658,19 +1755,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:21" ht="30.75">
       <c r="A54" s="19">
         <f>A52+1</f>
         <v>4</v>
       </c>
       <c r="B54" s="20" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D54" s="13" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="E54" s="12"/>
       <c r="F54">
@@ -1678,19 +1775,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:21" ht="43.15">
       <c r="A55" s="19">
         <f>A54+1</f>
         <v>5</v>
       </c>
       <c r="B55" s="20" t="s">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>1</v>
+        <v>84</v>
       </c>
       <c r="D55" s="13" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="E55" s="12"/>
       <c r="F55">
@@ -1698,13 +1795,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:21" ht="28.9">
       <c r="B56" s="5"/>
       <c r="C56" s="5" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="D56" s="13" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="E56" s="12"/>
       <c r="F56">
@@ -1712,13 +1809,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:21" ht="43.15">
       <c r="B57" s="5"/>
       <c r="C57" s="5" t="s">
-        <v>34</v>
+        <v>86</v>
       </c>
       <c r="D57" s="13" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="E57" s="12"/>
       <c r="F57">
@@ -1726,28 +1823,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:21" ht="28.9">
       <c r="A58" s="19">
         <v>7</v>
       </c>
       <c r="B58" s="20" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="D58" s="13" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="F58">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:21" ht="15.6">
       <c r="A59" s="5"/>
       <c r="B59" s="29" t="s">
-        <v>36</v>
+        <v>89</v>
       </c>
       <c r="C59" s="5"/>
       <c r="F59" s="10">
@@ -1755,10 +1852,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:21" ht="15.6">
       <c r="A60" s="5"/>
       <c r="B60" s="29" t="s">
-        <v>37</v>
+        <v>90</v>
       </c>
       <c r="C60" s="5"/>
       <c r="F60" s="10">
@@ -1781,7 +1878,7 @@
       <c r="T60" s="10"/>
       <c r="U60" s="10"/>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:21">
       <c r="A61" s="5"/>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
@@ -1831,24 +1928,24 @@
       <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="14.45"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fin seguridad y paquetes pl sql, rubrica final
</commit_message>
<xml_diff>
--- a/RubricaPlitix_SQLWarriors.xlsx
+++ b/RubricaPlitix_SQLWarriors.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28926"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alcaz\Git\ProyectoABD-SQLWarriors\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaime\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ADEAC8A1-B140-4250-A6ED-8ADF0DDF1408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F726A8-E779-4EC0-90CF-2ACB05A57C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="X7LfdmuZ3ss+actbBwJKlGQw0Mfe8mdGrYC6BLVbRaWZI0OVWK1VPKEuVw1nyVdQeaaH9MAmoO0Rse/4Wdr3PA==" workbookSaltValue="2gPJKYWhIGazIFYGx/RJog==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="15552" windowHeight="17376" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="106">
   <si>
     <t>Nombre del Grupo:</t>
   </si>
@@ -320,13 +320,52 @@
   </si>
   <si>
     <t>Columna1</t>
+  </si>
+  <si>
+    <t>Consultar los roles creados por el usuario dba_roles</t>
+  </si>
+  <si>
+    <t>Mostrar en el código del paquete PL/SQL</t>
+  </si>
+  <si>
+    <t>Añadir un commit y un rollback en los procedimientos</t>
+  </si>
+  <si>
+    <t>Ejecución de test con datos coherentes y verificar sus datos</t>
+  </si>
+  <si>
+    <t>Verificar que existen productos asociados a cuentas válidas (COUNT &gt; 0)</t>
+  </si>
+  <si>
+    <t>Todos los objetos siguen la convención de nombres en minúsculas (COUNT = 0 para nombres con mayús.)</t>
+  </si>
+  <si>
+    <t>Verificar los 3 objetos adicionales creados</t>
+  </si>
+  <si>
+    <t>Consultar dba_roles_privs</t>
+  </si>
+  <si>
+    <t>Consultar dba_profiles</t>
+  </si>
+  <si>
+    <t>Consultar dba_encrypted_columns</t>
+  </si>
+  <si>
+    <t>Consultar dba_role_privs</t>
+  </si>
+  <si>
+    <t>Comprobar que el modelo cumple con las restricciones semánticas (rangos válidos)</t>
+  </si>
+  <si>
+    <t>Comprobar las columnas obligatorias y las claves únicas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -514,7 +553,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -588,6 +627,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -901,20 +944,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C334588-D4EB-43EC-8424-5ED08F8B2503}">
   <dimension ref="A1:U61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="110" zoomScaleNormal="92" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="51.140625" customWidth="1"/>
-    <col min="3" max="3" width="46.140625" customWidth="1"/>
-    <col min="5" max="5" width="47.7109375" style="5" customWidth="1"/>
-    <col min="6" max="8" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="51.109375" customWidth="1"/>
+    <col min="3" max="3" width="46.109375" customWidth="1"/>
+    <col min="5" max="5" width="47.6640625" style="5" customWidth="1"/>
+    <col min="6" max="8" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="23.45">
+    <row r="1" spans="1:21" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="7"/>
       <c r="B1" s="7" t="s">
         <v>0</v>
@@ -924,7 +967,7 @@
       <c r="E1" s="8"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:21" ht="15.6">
+    <row r="2" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
@@ -934,7 +977,7 @@
       <c r="E2" s="15"/>
       <c r="F2" s="14"/>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -944,7 +987,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="28.9">
+    <row r="4" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -975,14 +1018,14 @@
       <c r="T4" s="3"/>
       <c r="U4" s="3"/>
     </row>
-    <row r="5" spans="1:21" ht="15.6">
+    <row r="5" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="18" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:21" ht="30.75">
+    <row r="6" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="19">
         <v>1</v>
       </c>
@@ -1003,7 +1046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="30.75">
+    <row r="7" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
         <v>12</v>
@@ -1019,7 +1062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="60.75">
+    <row r="8" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
         <v>14</v>
@@ -1035,7 +1078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="30.75">
+    <row r="9" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
         <v>16</v>
@@ -1051,7 +1094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="30.75">
+    <row r="10" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="19">
         <f>A6+1</f>
         <v>2</v>
@@ -1073,7 +1116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="30.75">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
         <v>21</v>
@@ -1089,7 +1132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="15.75">
+    <row r="12" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="19">
         <f>A10+1</f>
         <v>3</v>
@@ -1111,7 +1154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="15">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B13" s="5"/>
       <c r="C13" s="5" t="s">
         <v>26</v>
@@ -1127,7 +1170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="15.6">
+    <row r="14" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="19">
         <v>4</v>
       </c>
@@ -1140,26 +1183,30 @@
       <c r="D14" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="12"/>
+      <c r="E14" s="12" t="s">
+        <v>93</v>
+      </c>
       <c r="F14">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C15" s="21" t="s">
         <v>30</v>
       </c>
       <c r="D15" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="12"/>
+      <c r="E15" s="12" t="s">
+        <v>93</v>
+      </c>
       <c r="F15">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B16" s="5"/>
       <c r="C16" s="21" t="s">
         <v>31</v>
@@ -1167,13 +1214,15 @@
       <c r="D16" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="12"/>
+      <c r="E16" s="12" t="s">
+        <v>93</v>
+      </c>
       <c r="F16">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B17" s="5"/>
       <c r="C17" s="21" t="s">
         <v>32</v>
@@ -1181,13 +1230,15 @@
       <c r="D17" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="12"/>
+      <c r="E17" s="12" t="s">
+        <v>93</v>
+      </c>
       <c r="F17">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B18" s="5"/>
       <c r="C18" s="21" t="s">
         <v>33</v>
@@ -1195,13 +1246,15 @@
       <c r="D18" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="12"/>
+      <c r="E18" s="12" t="s">
+        <v>93</v>
+      </c>
       <c r="F18">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75">
+    <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="19">
         <v>5</v>
       </c>
@@ -1222,7 +1275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="30.75">
+    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="19">
         <f>A19+1</f>
         <v>6</v>
@@ -1244,7 +1297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="30.75">
+    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B21" s="5"/>
       <c r="C21" s="22" t="s">
         <v>40</v>
@@ -1260,7 +1313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="30.75">
+    <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B22" s="23"/>
       <c r="C22" s="22" t="s">
         <v>41</v>
@@ -1276,7 +1329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="30.75">
+    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" s="23"/>
       <c r="C23" s="22" t="s">
         <v>42</v>
@@ -1292,7 +1345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="30.75">
+    <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B24" s="23"/>
       <c r="C24" s="24" t="s">
         <v>43</v>
@@ -1308,7 +1361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="25.9" customHeight="1">
+    <row r="25" spans="1:6" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="23"/>
       <c r="C25" s="22" t="s">
         <v>45</v>
@@ -1324,7 +1377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C26" s="22" t="s">
         <v>46</v>
       </c>
@@ -1336,7 +1389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="25.9" customHeight="1">
+    <row r="27" spans="1:6" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="23"/>
       <c r="C27" s="22" t="s">
         <v>47</v>
@@ -1352,7 +1405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="25.9" customHeight="1">
+    <row r="28" spans="1:6" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="23"/>
       <c r="C28" s="22" t="s">
         <v>48</v>
@@ -1368,7 +1421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.75">
+    <row r="29" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="19">
         <f>A20+1</f>
         <v>7</v>
@@ -1390,7 +1443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="28.9">
+    <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="19">
         <f>A29+1</f>
         <v>8</v>
@@ -1404,13 +1457,15 @@
       <c r="D30" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E30" s="12"/>
+      <c r="E30" s="12" t="s">
+        <v>95</v>
+      </c>
       <c r="F30">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.6">
+    <row r="31" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="19">
         <f>A30+1</f>
         <v>9</v>
@@ -1424,13 +1479,15 @@
       <c r="D31" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E31" s="12"/>
+      <c r="E31" s="12" t="s">
+        <v>94</v>
+      </c>
       <c r="F31">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.6">
+    <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="19">
         <f>A31+1</f>
         <v>10</v>
@@ -1440,15 +1497,17 @@
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="E32" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>96</v>
+      </c>
       <c r="F32">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" ht="15.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="19">
         <f>A32+1</f>
         <v>11</v>
@@ -1470,87 +1529,97 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="30.75">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B34" s="5"/>
       <c r="C34" s="5" t="s">
         <v>60</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="E34" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>100</v>
+      </c>
       <c r="F34">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" ht="28.9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B35" s="5"/>
       <c r="C35" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="E35" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="E35" s="31" t="s">
+        <v>103</v>
+      </c>
       <c r="F35">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B36" s="5"/>
       <c r="C36" s="5" t="s">
         <v>62</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="E36" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>103</v>
+      </c>
       <c r="F36">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B37" s="5"/>
       <c r="C37" s="5" t="s">
         <v>63</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="E37" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>101</v>
+      </c>
       <c r="F37">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B38" s="5"/>
       <c r="C38" s="5" t="s">
         <v>64</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="E38" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="E38" s="31" t="s">
+        <v>102</v>
+      </c>
       <c r="F38">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="9"/>
       <c r="F39" s="11">
         <f>SUM(F6:F38)/COUNT(F6:F38)*2</f>
-        <v>1.6363636363636365</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" ht="23.45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B40" s="25" t="s">
         <v>65</v>
       </c>
@@ -1572,7 +1641,7 @@
       <c r="S40" s="10"/>
       <c r="T40" s="10"/>
     </row>
-    <row r="41" spans="1:20" ht="23.45">
+    <row r="41" spans="1:20" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B41" s="25" t="s">
         <v>66</v>
       </c>
@@ -1580,7 +1649,7 @@
       <c r="D41" s="5"/>
       <c r="E41" s="9"/>
     </row>
-    <row r="42" spans="1:20" ht="23.45">
+    <row r="42" spans="1:20" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B42" s="25" t="s">
         <v>67</v>
       </c>
@@ -1588,17 +1657,17 @@
       <c r="D42" s="5"/>
       <c r="E42" s="9"/>
     </row>
-    <row r="43" spans="1:20">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="9"/>
     </row>
-    <row r="44" spans="1:20">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B44" s="5"/>
       <c r="E44" s="9"/>
     </row>
-    <row r="45" spans="1:20" ht="15.6">
+    <row r="45" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="19">
         <v>1</v>
       </c>
@@ -1619,7 +1688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="15.6">
+    <row r="46" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="17"/>
       <c r="B46" s="26"/>
       <c r="C46" s="5" t="s">
@@ -1636,7 +1705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="15.6">
+    <row r="47" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="17"/>
       <c r="B47" s="26"/>
       <c r="C47" s="5" t="s">
@@ -1653,7 +1722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="30.75">
+    <row r="48" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="17"/>
       <c r="B48" s="26"/>
       <c r="C48" s="5" t="s">
@@ -1670,7 +1739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:21" ht="30.75">
+    <row r="49" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="17"/>
       <c r="B49" s="26"/>
       <c r="C49" s="5" t="s">
@@ -1687,7 +1756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:21" ht="15.75">
+    <row r="50" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="19">
         <v>2</v>
       </c>
@@ -1708,7 +1777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="15.6">
+    <row r="51" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="26"/>
       <c r="B51" s="26"/>
       <c r="C51" s="5" t="s">
@@ -1725,7 +1794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:21" ht="43.15">
+    <row r="52" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A52" s="19">
         <v>3</v>
       </c>
@@ -1736,29 +1805,33 @@
         <v>79</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="E52" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="E52" s="12" t="s">
+        <v>104</v>
+      </c>
       <c r="F52">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B53" s="5"/>
       <c r="C53" s="28" t="s">
         <v>80</v>
       </c>
       <c r="D53" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="E53" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="E53" s="12" t="s">
+        <v>105</v>
+      </c>
       <c r="F53">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:21" ht="30.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="19">
         <f>A52+1</f>
         <v>4</v>
@@ -1780,7 +1853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:21" ht="43.15">
+    <row r="55" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" s="19">
         <f>A54+1</f>
         <v>5</v>
@@ -1792,43 +1865,49 @@
         <v>85</v>
       </c>
       <c r="D55" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="E55" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="E55" s="12" t="s">
+        <v>97</v>
+      </c>
       <c r="F55">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:21" ht="28.9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B56" s="5"/>
       <c r="C56" s="5" t="s">
         <v>86</v>
       </c>
       <c r="D56" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="E56" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="E56" s="12" t="s">
+        <v>98</v>
+      </c>
       <c r="F56">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:21" ht="43.15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B57" s="5"/>
       <c r="C57" s="5" t="s">
         <v>87</v>
       </c>
       <c r="D57" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="E57" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="E57" s="12" t="s">
+        <v>99</v>
+      </c>
       <c r="F57">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:21" ht="28.9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A58" s="19">
         <v>7</v>
       </c>
@@ -1839,14 +1918,14 @@
         <v>89</v>
       </c>
       <c r="D58" s="13" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="F58">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:21" ht="15.6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="5"/>
       <c r="B59" s="29" t="s">
         <v>90</v>
@@ -1854,10 +1933,10 @@
       <c r="C59" s="5"/>
       <c r="F59" s="10">
         <f>SUM(F45:F58)/COUNT(F45:F58)*2</f>
-        <v>1.1428571428571428</v>
-      </c>
-    </row>
-    <row r="60" spans="1:21" ht="15.6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="5"/>
       <c r="B60" s="29" t="s">
         <v>91</v>
@@ -1865,7 +1944,7 @@
       <c r="C60" s="5"/>
       <c r="F60" s="10">
         <f>F59+F39</f>
-        <v>2.779220779220779</v>
+        <v>4</v>
       </c>
       <c r="G60" s="10"/>
       <c r="H60" s="10"/>
@@ -1883,7 +1962,7 @@
       <c r="T60" s="10"/>
       <c r="U60" s="10"/>
     </row>
-    <row r="61" spans="1:21">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A61" s="5"/>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
@@ -1933,22 +2012,22 @@
       <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>57</v>
       </c>

</xml_diff>